<commit_message>
Redid Some Graphs, added results to spreadsheets of IC Study
</commit_message>
<xml_diff>
--- a/results/spreadsheets/Results Overview.xlsx
+++ b/results/spreadsheets/Results Overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9696" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9690" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Burgers Summary" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
   <si>
     <t>Method</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>Allen-Cahn</t>
+  </si>
+  <si>
+    <t>no resample</t>
+  </si>
+  <si>
+    <t>wu</t>
+  </si>
+  <si>
+    <t>uxt</t>
+  </si>
+  <si>
+    <t>n=1000</t>
   </si>
 </sst>
 </file>
@@ -981,6 +993,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2142,6 +2155,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2300,6 +2314,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5362,6 +5377,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5473,6 +5489,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6721,6 +6738,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6832,6 +6850,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7409,6 +7428,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7515,6 +7535,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8093,6 +8114,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8714,6 +8736,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19339,35 +19362,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="27"/>
-    <col min="5" max="5" width="18.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="27"/>
+    <col min="5" max="5" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="57" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="16" width="9.88671875" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" style="2" customWidth="1"/>
-    <col min="18" max="20" width="9.88671875" customWidth="1"/>
-    <col min="21" max="21" width="9.88671875" style="2" customWidth="1"/>
-    <col min="22" max="23" width="9.88671875" customWidth="1"/>
-    <col min="24" max="24" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="11.6640625" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" style="2" customWidth="1"/>
-    <col min="30" max="31" width="11.6640625" customWidth="1"/>
-    <col min="34" max="34" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="2" customWidth="1"/>
+    <col min="18" max="20" width="9.85546875" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="2" customWidth="1"/>
+    <col min="22" max="23" width="9.85546875" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="11.7109375" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" style="2" customWidth="1"/>
+    <col min="30" max="31" width="11.7109375" customWidth="1"/>
+    <col min="34" max="34" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
@@ -19408,7 +19431,7 @@
       <c r="AG1" s="91"/>
       <c r="AH1" s="66"/>
     </row>
-    <row r="2" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -19494,7 +19517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -19576,7 +19599,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
@@ -19669,7 +19692,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>43</v>
       </c>
@@ -19763,7 +19786,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>53</v>
       </c>
@@ -19856,7 +19879,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>5</v>
       </c>
@@ -19950,7 +19973,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="I8" s="3" t="s">
         <v>83</v>
       </c>
@@ -20028,7 +20051,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -20109,7 +20132,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B10" s="53" t="s">
         <v>0</v>
       </c>
@@ -20196,7 +20219,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>4</v>
       </c>
@@ -20286,7 +20309,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>43</v>
       </c>
@@ -20320,7 +20343,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>44</v>
       </c>
@@ -20349,7 +20372,7 @@
       <c r="X13" s="21"/>
       <c r="Z13" s="4"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -20385,7 +20408,7 @@
       <c r="X14" s="21"/>
       <c r="Z14" s="4"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
         <v>21</v>
       </c>
@@ -20407,7 +20430,7 @@
       <c r="I15" s="3"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="30"/>
@@ -20426,7 +20449,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="4"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="7" t="s">
         <v>0</v>
@@ -20461,7 +20484,7 @@
       <c r="Y17" s="21"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="3" t="s">
         <v>58</v>
@@ -20479,7 +20502,7 @@
         <v>4.2764451039324939E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="3" t="s">
         <v>67</v>
@@ -20501,7 +20524,7 @@
       <c r="T19" s="27"/>
       <c r="X19" s="27"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
@@ -20531,7 +20554,7 @@
       </c>
       <c r="AC20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="3" t="s">
         <v>56</v>
@@ -20612,7 +20635,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="3" t="s">
         <v>61</v>
@@ -20695,7 +20718,7 @@
         <v>9.152299398574554</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="5" t="s">
         <v>68</v>
@@ -20788,7 +20811,7 @@
         <v>6.7045363062052399</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>69</v>
       </c>
@@ -20883,7 +20906,7 @@
         <v>6.6425910523103218</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>69</v>
       </c>
@@ -20978,7 +21001,7 @@
         <v>6.7834730540950963</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>69</v>
       </c>
@@ -21071,7 +21094,7 @@
         <v>6.2882083724750286</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>15</v>
       </c>
@@ -21166,7 +21189,7 @@
         <v>6.8082700717607985</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>15</v>
       </c>
@@ -21261,7 +21284,7 @@
         <v>8.9498643226702921</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>26</v>
       </c>
@@ -21357,7 +21380,7 @@
         <v>7.6351215843041622</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>26</v>
       </c>
@@ -21459,7 +21482,7 @@
         <v>6.9676561199558948</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>26</v>
       </c>
@@ -21483,7 +21506,7 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>77</v>
       </c>
@@ -21507,7 +21530,7 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>76</v>
       </c>
@@ -21531,30 +21554,30 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -21574,7 +21597,7 @@
         <v>2.9546964738979273E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -21594,7 +21617,7 @@
         <v>8.0034560916735224E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -21614,7 +21637,7 @@
         <v>1.9433491595482804E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -21634,7 +21657,7 @@
         <v>2.6571175145016925E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>40</v>
       </c>
@@ -21648,7 +21671,7 @@
         <v>4.3291963926304087E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>50</v>
       </c>
@@ -21662,7 +21685,7 @@
         <v>2.8040200083282672E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D47" s="27">
         <f>((4*D45)+(5*D46))/9</f>
         <v>2.4681735990621423</v>
@@ -21679,7 +21702,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S48" t="s">
         <v>106</v>
       </c>
@@ -21687,7 +21710,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J52">
         <v>1</v>
       </c>
@@ -21695,7 +21718,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J53">
         <v>2</v>
       </c>
@@ -21703,7 +21726,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J55" t="s">
         <v>110</v>
       </c>
@@ -21732,13 +21755,13 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C1" s="177" t="s">
         <v>1</v>
       </c>
@@ -21764,7 +21787,7 @@
       <c r="S1" s="177"/>
       <c r="T1" s="166"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="174" t="s">
         <v>132</v>
       </c>
@@ -21790,7 +21813,7 @@
       <c r="S2" s="176"/>
       <c r="T2" s="167"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -21852,7 +21875,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>123</v>
       </c>
@@ -21914,7 +21937,7 @@
         <v>3.4755864065810715E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -21976,7 +21999,7 @@
         <v>8.0034560916735224E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="62" t="s">
         <v>36</v>
       </c>
@@ -22038,7 +22061,7 @@
         <v>4.136445436834629E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
@@ -22116,19 +22139,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="68"/>
       <c r="C2" s="68" t="s">
         <v>135</v>
@@ -22136,8 +22159,11 @@
       <c r="D2" s="68" t="s">
         <v>136</v>
       </c>
+      <c r="E2" s="68" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="68" t="s">
         <v>133</v>
       </c>
@@ -22147,8 +22173,11 @@
       <c r="D3" s="68">
         <v>2000</v>
       </c>
+      <c r="E3" s="68">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="68" t="s">
         <v>125</v>
       </c>
@@ -22158,8 +22187,11 @@
       <c r="D4" s="171">
         <v>1.5723195585830318E-4</v>
       </c>
+      <c r="E4" s="171">
+        <v>1.7229788549101105E-4</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="68" t="s">
         <v>134</v>
       </c>
@@ -22169,6 +22201,24 @@
       <c r="D5" s="171">
         <v>1.8006410808587452E-3</v>
       </c>
+      <c r="E5" s="171">
+        <v>3.5516194937243476E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="27"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="75"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="27"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="75"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="27"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22177,20 +22227,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C1" s="174" t="s">
         <v>38</v>
       </c>
@@ -22217,7 +22268,7 @@
       <c r="R1" s="179"/>
       <c r="S1" s="127"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -22276,7 +22327,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>123</v>
       </c>
@@ -22325,7 +22376,7 @@
       </c>
       <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>123</v>
       </c>
@@ -22374,7 +22425,7 @@
       </c>
       <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -22423,7 +22474,7 @@
       </c>
       <c r="S5" s="16"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -22472,7 +22523,7 @@
       </c>
       <c r="S6" s="16"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
@@ -22521,7 +22572,7 @@
       </c>
       <c r="S7" s="18"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -22570,7 +22621,7 @@
       </c>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -22619,7 +22670,7 @@
       </c>
       <c r="S9" s="16"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -22667,8 +22718,11 @@
         <v>1.3152318182401298E-3</v>
       </c>
       <c r="S10" s="16"/>
+      <c r="U10" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>119</v>
       </c>
@@ -22716,8 +22770,20 @@
         <v>6.7811121786916645E-3</v>
       </c>
       <c r="S11" s="18"/>
+      <c r="U11" t="s">
+        <v>137</v>
+      </c>
+      <c r="V11" s="27">
+        <v>5.6862138099299395</v>
+      </c>
+      <c r="W11" s="98">
+        <v>1.7229788549101105E-4</v>
+      </c>
+      <c r="X11" s="75">
+        <v>1.2751155160426627E-5</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -22765,8 +22831,20 @@
         <v>6.2504146170973942E-3</v>
       </c>
       <c r="S12" s="17"/>
+      <c r="U12" t="s">
+        <v>138</v>
+      </c>
+      <c r="V12" s="27">
+        <v>4.3473319473372438</v>
+      </c>
+      <c r="W12" s="98">
+        <v>3.5516194937243476E-3</v>
+      </c>
+      <c r="X12" s="75">
+        <v>6.393800033238117E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>126</v>
       </c>
@@ -22814,8 +22892,20 @@
         <v>2.6276170301547694E-3</v>
       </c>
       <c r="S13" s="16"/>
+      <c r="U13" t="s">
+        <v>139</v>
+      </c>
+      <c r="V13" s="27">
+        <v>4.147073000231039</v>
+      </c>
+      <c r="W13" s="98">
+        <v>7.7184528176727019E-3</v>
+      </c>
+      <c r="X13" s="75">
+        <v>4.8516322387169115E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>126</v>
       </c>
@@ -22887,9 +22977,9 @@
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>124</v>
       </c>
@@ -22897,7 +22987,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -22917,7 +23007,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -22937,7 +23027,7 @@
         <v>0.85011200669771603</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>10000</v>
       </c>
@@ -22957,7 +23047,7 @@
         <v>5.31436755056323E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>15000</v>
       </c>
@@ -22977,7 +23067,7 @@
         <v>9.2074255800552395E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>15000</v>
       </c>
@@ -22997,7 +23087,7 @@
         <v>9.2074255800552395E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>20000</v>
       </c>
@@ -23017,7 +23107,7 @@
         <v>9.2026244499063793E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>30000</v>
       </c>
@@ -23037,7 +23127,7 @@
         <v>1.6422225023270001E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>40000</v>
       </c>
@@ -23057,7 +23147,7 @@
         <v>6.5116946846434505E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>50000</v>
       </c>
@@ -23077,7 +23167,7 @@
         <v>3.78738507059801E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>60000</v>
       </c>
@@ -23097,7 +23187,7 @@
         <v>2.5588131327053299E-7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>70000</v>
       </c>
@@ -23117,7 +23207,7 @@
         <v>2.01544925767743E-7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>80000</v>
       </c>
@@ -23137,7 +23227,7 @@
         <v>1.60919824370242E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>90000</v>
       </c>
@@ -23157,7 +23247,7 @@
         <v>1.3703947909155701E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>100000</v>
       </c>
@@ -23177,7 +23267,7 @@
         <v>1.2055444704729601E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>110000</v>
       </c>
@@ -23197,7 +23287,7 @@
         <v>1.0916885325234201E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>120000</v>
       </c>
@@ -23217,7 +23307,7 @@
         <v>9.8362379222636101E-8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>130000</v>
       </c>
@@ -23237,7 +23327,7 @@
         <v>9.0630800965466194E-8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>140000</v>
       </c>
@@ -23257,7 +23347,7 @@
         <v>8.3526053142033499E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>150000</v>
       </c>
@@ -23277,7 +23367,7 @@
         <v>7.7554911775123797E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>160000</v>
       </c>
@@ -23297,7 +23387,7 @@
         <v>7.2563057526737306E-8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>170000</v>
       </c>
@@ -23317,7 +23407,7 @@
         <v>6.8443994238359405E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>180000</v>
       </c>
@@ -23337,7 +23427,7 @@
         <v>6.4264250140045006E-8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>190000</v>
       </c>
@@ -23357,7 +23447,7 @@
         <v>6.09572502478564E-8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>200000</v>
       </c>
@@ -23377,7 +23467,7 @@
         <v>5.7892290025897999E-8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>210000</v>
       </c>
@@ -23397,7 +23487,7 @@
         <v>5.4672630037131797E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>220000</v>
       </c>
@@ -23417,7 +23507,7 @@
         <v>5.1775103843723499E-8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>230000</v>
       </c>
@@ -23437,7 +23527,7 @@
         <v>4.91213799705783E-8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>240000</v>
       </c>
@@ -23457,7 +23547,7 @@
         <v>4.7343496261112102E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>250000</v>
       </c>
@@ -23477,7 +23567,7 @@
         <v>4.62263188776967E-8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>260000</v>
       </c>
@@ -23497,7 +23587,7 @@
         <v>4.5214384184331099E-8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>270000</v>
       </c>
@@ -23517,7 +23607,7 @@
         <v>4.4408856549915903E-8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>280000</v>
       </c>
@@ -23537,7 +23627,7 @@
         <v>4.3553581401780903E-8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>290000</v>
       </c>
@@ -23557,7 +23647,7 @@
         <v>4.2756909490131E-8</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>300000</v>
       </c>
@@ -23577,7 +23667,7 @@
         <v>4.19906114844401E-8</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>310000</v>
       </c>
@@ -23597,7 +23687,7 @@
         <v>4.1422235425819097E-8</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>320000</v>
       </c>
@@ -23617,7 +23707,7 @@
         <v>4.0921967146942303E-8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>330000</v>
       </c>
@@ -23637,7 +23727,7 @@
         <v>4.0449729646364203E-8</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>340000</v>
       </c>
@@ -23657,7 +23747,7 @@
         <v>3.9902964011607798E-8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>350000</v>
       </c>
@@ -23677,7 +23767,7 @@
         <v>3.9346560906847403E-8</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>360000</v>
       </c>
@@ -23697,7 +23787,7 @@
         <v>3.8869277375702702E-8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>370000</v>
       </c>
@@ -23717,7 +23807,7 @@
         <v>3.8451817599629E-8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>380000</v>
       </c>
@@ -23737,7 +23827,7 @@
         <v>3.8028031615645001E-8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>390000</v>
       </c>
@@ -23757,7 +23847,7 @@
         <v>3.74916953123856E-8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>400000</v>
       </c>
@@ -23777,7 +23867,7 @@
         <v>3.71353117629118E-8</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>410000</v>
       </c>
@@ -23797,7 +23887,7 @@
         <v>3.6781021536088701E-8</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>420000</v>
       </c>
@@ -23817,7 +23907,7 @@
         <v>3.6450534489262599E-8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>430000</v>
       </c>
@@ -23837,7 +23927,7 @@
         <v>3.61712343379565E-8</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>430965</v>
       </c>
@@ -23871,20 +23961,20 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="2"/>
-    <col min="9" max="9" width="9.109375" style="57"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.140625" style="57"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="27"/>
-    <col min="16" max="17" width="9.109375" style="2"/>
+    <col min="15" max="15" width="9.140625" style="27"/>
+    <col min="16" max="17" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -23895,7 +23985,7 @@
       </c>
       <c r="P2" s="49"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -23936,7 +24026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
@@ -23980,7 +24070,7 @@
         <v>4.2846792135832187E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -24024,7 +24114,7 @@
         <v>3.2581148646597212E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -24068,7 +24158,7 @@
         <v>9.5817494854836E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
@@ -24091,7 +24181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
@@ -24112,7 +24202,7 @@
       </c>
       <c r="H8" s="56"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
@@ -24132,7 +24222,7 @@
         <v>2.048560416308142E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
@@ -24152,7 +24242,7 @@
         <v>1.9147480743070145E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
@@ -24172,7 +24262,7 @@
         <v>1.6975951420033131E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
@@ -24192,7 +24282,7 @@
         <v>1.5400170959997073E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -24212,7 +24302,7 @@
         <v>1.9083453268669933E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
@@ -24235,7 +24325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
@@ -24258,7 +24348,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -24281,7 +24371,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="33" t="s">
         <v>26</v>
       </c>
@@ -24301,7 +24391,7 @@
         <v>1.7706268644262122E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
         <v>26</v>
       </c>
@@ -24321,7 +24411,7 @@
         <v>1.5978325040835362E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="35" t="s">
         <v>26</v>
       </c>
@@ -24341,16 +24431,16 @@
         <v>1.3070070314676611E-4</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E20" s="27"/>
       <c r="F20" s="49"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="E21" s="27"/>
       <c r="F21" s="49"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
         <v>0</v>
@@ -24368,7 +24458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>36</v>
       </c>
@@ -24391,7 +24481,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
@@ -24411,7 +24501,7 @@
         <v>2.1633824782506494E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
@@ -24434,7 +24524,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
@@ -24457,7 +24547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>36</v>
       </c>
@@ -24480,7 +24570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="58" t="s">
         <v>62</v>
       </c>
@@ -24490,7 +24580,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="41"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="60" t="s">
         <v>63</v>
       </c>
@@ -24500,7 +24590,7 @@
       <c r="F29" s="20"/>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="35" t="s">
         <v>64</v>
       </c>
@@ -24510,13 +24600,13 @@
       <c r="F30" s="22"/>
       <c r="G30" s="26"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E32" s="27"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="42" t="s">
         <v>59</v>
       </c>
@@ -24536,7 +24626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>21</v>
       </c>
@@ -24559,7 +24649,7 @@
         <v>2.3492443632009731E-4</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>21</v>
       </c>
@@ -24582,7 +24672,7 @@
         <v>3.6258165586535845E-4</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="59" t="s">
         <v>54</v>
       </c>
@@ -24605,7 +24695,7 @@
         <v>4.2764451039324939E-4</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="58" t="s">
         <v>55</v>
       </c>
@@ -24628,7 +24718,7 @@
         <v>6.1133261759914058E-4</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="58" t="s">
         <v>55</v>
       </c>

</xml_diff>